<commit_message>
side by side is ok
</commit_message>
<xml_diff>
--- a/source/burgerKing/src/main/resources/template/Guest Is King.xlsx
+++ b/source/burgerKing/src/main/resources/template/Guest Is King.xlsx
@@ -1676,10 +1676,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>${heads.date}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>${heads.manager}</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1750,10 +1746,6 @@
   </si>
   <si>
     <t>${modules.qingjie_waibu.questions.C01.testDetailInfo.fieldInfos.SCORE}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${modules.qingjie_waibu.questions.C01.testDetailInfo.fieldInfos.DESC}</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -3214,6 +3206,14 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;jt:forEach copyRight="true" items="${modules.pingguzongjie.questions.pg_guanzhu.testDetailInfo.evidence}" var="ev"&gt;&lt;jt:hyperlink type="url" address="${ev.address}" value="${ev.value}"/&gt;&lt;/jt:forEach&gt;</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>${heads.date}</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>${modules.qingjie_waibu.questions.C01.testDetailInfo.fieldInfos.DESC}</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -3515,19 +3515,22 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3542,6 +3545,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3549,6 +3555,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3580,24 +3598,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3909,7 +3909,7 @@
   <dimension ref="A1:U82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U53" sqref="U53"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3919,162 +3919,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="28.35" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
     </row>
     <row r="2" spans="1:21" ht="15">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="18" t="s">
+        <v>580</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="20"/>
+      <c r="P2" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="U2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15">
+      <c r="A3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="U2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15">
-      <c r="A3" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="P3" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="17" t="s">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" t="s">
+        <v>155</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15">
+      <c r="A4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" t="s">
-        <v>157</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15">
-      <c r="A4" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
       <c r="U4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
       <c r="U5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="16.5">
-      <c r="A6" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="A6" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="4" t="s">
         <v>74</v>
       </c>
@@ -4090,15 +4090,15 @@
       <c r="L6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="S6" s="7"/>
     </row>
@@ -4106,304 +4106,304 @@
       <c r="A7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="38" t="s">
-        <v>516</v>
-      </c>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
+      <c r="M7" s="21" t="s">
+        <v>581</v>
+      </c>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:21" ht="30" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="38" t="s">
-        <v>517</v>
-      </c>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
     </row>
     <row r="9" spans="1:21" ht="30" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="38" t="s">
-        <v>518</v>
-      </c>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
     </row>
     <row r="10" spans="1:21" ht="30" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="38" t="s">
-        <v>519</v>
-      </c>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:21" ht="30" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="38" t="s">
-        <v>520</v>
-      </c>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
     </row>
     <row r="12" spans="1:21" ht="30" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="38" t="s">
-        <v>521</v>
-      </c>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
     </row>
     <row r="13" spans="1:21" ht="30" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="M13" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="38" t="s">
-        <v>522</v>
-      </c>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
     </row>
     <row r="14" spans="1:21" ht="15.75">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="S14" s="35"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="S14" s="13"/>
     </row>
     <row r="15" spans="1:21" ht="16.5">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="4" t="s">
         <v>74</v>
       </c>
@@ -4419,15 +4419,15 @@
       <c r="L15" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="34" t="s">
-        <v>511</v>
+      <c r="R15" s="12" t="s">
+        <v>509</v>
       </c>
       <c r="S15" s="7"/>
     </row>
@@ -4435,304 +4435,304 @@
       <c r="A16" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="M16" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="38" t="s">
-        <v>523</v>
-      </c>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="16" t="s">
+        <v>521</v>
+      </c>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
     </row>
     <row r="17" spans="1:19" ht="30" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="38" t="s">
-        <v>529</v>
-      </c>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
+        <v>201</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:19" ht="30" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="38" t="s">
-        <v>528</v>
-      </c>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:19" ht="30" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
       <c r="H19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="M19" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="M19" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="38" t="s">
-        <v>527</v>
-      </c>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
     </row>
     <row r="20" spans="1:19" ht="30" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
       <c r="H20" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="M20" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="M20" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="38" t="s">
-        <v>526</v>
-      </c>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
     </row>
     <row r="21" spans="1:19" ht="30" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="M21" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="38" t="s">
-        <v>525</v>
-      </c>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
     </row>
     <row r="22" spans="1:19" ht="30" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="K22" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="M22" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="L22" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="M22" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="38" t="s">
-        <v>524</v>
-      </c>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
     </row>
     <row r="23" spans="1:19" ht="15.75">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="S23" s="35"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" ht="16.5">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
       <c r="H24" s="4" t="s">
         <v>74</v>
       </c>
@@ -4748,15 +4748,15 @@
       <c r="L24" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M24" s="12" t="s">
+      <c r="M24" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
       <c r="Q24" s="7"/>
-      <c r="R24" s="34" t="s">
-        <v>512</v>
+      <c r="R24" s="12" t="s">
+        <v>510</v>
       </c>
       <c r="S24" s="7"/>
     </row>
@@ -4764,304 +4764,304 @@
       <c r="A25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
       <c r="H25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="M25" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="M25" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="38" t="s">
-        <v>530</v>
-      </c>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="16" t="s">
+        <v>528</v>
+      </c>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
     </row>
     <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
       <c r="H26" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="L26" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="M26" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="L26" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="M26" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="38" t="s">
-        <v>531</v>
-      </c>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="M27" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="L27" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="M27" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="38" t="s">
-        <v>532</v>
-      </c>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
     </row>
     <row r="28" spans="1:19" ht="30" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="M28" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="M28" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="38" t="s">
-        <v>533</v>
-      </c>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="16" t="s">
+        <v>531</v>
+      </c>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
     </row>
     <row r="29" spans="1:19" ht="30" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="M29" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="L29" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="M29" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="38" t="s">
-        <v>534</v>
-      </c>
-      <c r="R29" s="38"/>
-      <c r="S29" s="38"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
     </row>
     <row r="30" spans="1:19" ht="30" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
       <c r="H30" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="M30" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="38" t="s">
-        <v>535</v>
-      </c>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
     </row>
     <row r="31" spans="1:19" ht="30" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
       <c r="H31" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="M31" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="L31" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="M31" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="38" t="s">
-        <v>536</v>
-      </c>
-      <c r="R31" s="38"/>
-      <c r="S31" s="38"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="16" t="s">
+        <v>534</v>
+      </c>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
     </row>
     <row r="32" spans="1:19" ht="15.75">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="S32" s="35"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="S32" s="13"/>
     </row>
     <row r="33" spans="1:19" ht="16.5">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
       <c r="H33" s="1" t="s">
         <v>74</v>
       </c>
@@ -5077,281 +5077,281 @@
       <c r="L33" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M33" s="20" t="s">
+      <c r="M33" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="22"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="24"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="S33" s="36"/>
+        <v>511</v>
+      </c>
+      <c r="S33" s="14"/>
     </row>
     <row r="34" spans="1:19" ht="30" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
       <c r="H34" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="M34" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="38" t="s">
-        <v>538</v>
-      </c>
-      <c r="R34" s="38"/>
-      <c r="S34" s="38"/>
+      <c r="M34" s="21" t="s">
+        <v>535</v>
+      </c>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
     </row>
     <row r="35" spans="1:19" ht="30" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
       <c r="H35" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="L35" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="M35" s="21" t="s">
         <v>397</v>
       </c>
-      <c r="L35" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="M35" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="38" t="s">
-        <v>539</v>
-      </c>
-      <c r="R35" s="38"/>
-      <c r="S35" s="38"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
     </row>
     <row r="36" spans="1:19" ht="30" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
       <c r="H36" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="M36" s="21" t="s">
         <v>403</v>
       </c>
-      <c r="L36" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="M36" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="38" t="s">
-        <v>540</v>
-      </c>
-      <c r="R36" s="38"/>
-      <c r="S36" s="38"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
     </row>
     <row r="37" spans="1:19" ht="30" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
       <c r="H37" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="L37" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="M37" s="21" t="s">
         <v>409</v>
       </c>
-      <c r="L37" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="M37" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="38" t="s">
-        <v>541</v>
-      </c>
-      <c r="R37" s="38"/>
-      <c r="S37" s="38"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
     </row>
     <row r="38" spans="1:19" ht="30" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="M38" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="L38" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="M38" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="38" t="s">
-        <v>542</v>
-      </c>
-      <c r="R38" s="38"/>
-      <c r="S38" s="38"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
     </row>
     <row r="39" spans="1:19" ht="30" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
       <c r="H39" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="M39" s="21" t="s">
         <v>421</v>
       </c>
-      <c r="L39" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="M39" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="38" t="s">
-        <v>543</v>
-      </c>
-      <c r="R39" s="38"/>
-      <c r="S39" s="38"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="16" t="s">
+        <v>541</v>
+      </c>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
     </row>
     <row r="40" spans="1:19" ht="15.75">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="S40" s="35"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="S40" s="13"/>
     </row>
     <row r="41" spans="1:19" ht="16.5">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
       <c r="H41" s="4" t="s">
         <v>74</v>
       </c>
@@ -5367,15 +5367,15 @@
       <c r="L41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M41" s="12" t="s">
+      <c r="M41" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
       <c r="Q41" s="7"/>
-      <c r="R41" s="34" t="s">
-        <v>514</v>
+      <c r="R41" s="12" t="s">
+        <v>512</v>
       </c>
       <c r="S41" s="7"/>
     </row>
@@ -5383,265 +5383,265 @@
       <c r="A42" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
       <c r="H42" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="K42" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="M42" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="38" t="s">
-        <v>545</v>
-      </c>
-      <c r="R42" s="38"/>
-      <c r="S42" s="38"/>
+      <c r="M42" s="21" t="s">
+        <v>542</v>
+      </c>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="16" t="s">
+        <v>543</v>
+      </c>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
     </row>
     <row r="43" spans="1:19" ht="30" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
       <c r="H43" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="J43" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="L43" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="M43" s="21" t="s">
         <v>362</v>
       </c>
-      <c r="L43" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="M43" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="38" t="s">
-        <v>546</v>
-      </c>
-      <c r="R43" s="38"/>
-      <c r="S43" s="38"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="16" t="s">
+        <v>544</v>
+      </c>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
     </row>
     <row r="44" spans="1:19" ht="30" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
       <c r="H44" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J44" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="K44" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="M44" s="21" t="s">
         <v>368</v>
       </c>
-      <c r="L44" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="M44" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="38" t="s">
-        <v>547</v>
-      </c>
-      <c r="R44" s="38"/>
-      <c r="S44" s="38"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
     </row>
     <row r="45" spans="1:19" ht="30" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
       <c r="H45" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="K45" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="M45" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="L45" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="M45" s="11" t="s">
-        <v>376</v>
-      </c>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="38" t="s">
-        <v>548</v>
-      </c>
-      <c r="R45" s="38"/>
-      <c r="S45" s="38"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
     </row>
     <row r="46" spans="1:19" ht="30" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
       <c r="H46" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="K46" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="M46" s="21" t="s">
         <v>380</v>
       </c>
-      <c r="L46" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="M46" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="38" t="s">
-        <v>549</v>
-      </c>
-      <c r="R46" s="38"/>
-      <c r="S46" s="38"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
     </row>
     <row r="47" spans="1:19" ht="30" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="B47" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
       <c r="H47" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="K47" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="M47" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="L47" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="M47" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="38" t="s">
-        <v>550</v>
-      </c>
-      <c r="R47" s="38"/>
-      <c r="S47" s="38"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="16" t="s">
+        <v>548</v>
+      </c>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
     </row>
     <row r="48" spans="1:19" ht="15.75">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="25"/>
-      <c r="S48" s="35"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="S48" s="13"/>
     </row>
     <row r="49" spans="1:19" ht="16.5">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
       <c r="H49" s="1" t="s">
         <v>74</v>
       </c>
@@ -5657,515 +5657,515 @@
       <c r="L49" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M49" s="20" t="s">
+      <c r="M49" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
-      <c r="P49" s="22"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="24"/>
       <c r="Q49" s="10"/>
       <c r="R49" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="S49" s="36"/>
+        <v>507</v>
+      </c>
+      <c r="S49" s="14"/>
     </row>
     <row r="50" spans="1:19" ht="30" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
+      <c r="B50" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
       <c r="H50" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="K50" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="M50" s="25" t="s">
         <v>339</v>
       </c>
-      <c r="L50" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="M50" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="15"/>
-      <c r="Q50" s="38" t="s">
-        <v>551</v>
-      </c>
-      <c r="R50" s="38"/>
-      <c r="S50" s="38"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
+      <c r="P50" s="27"/>
+      <c r="Q50" s="16" t="s">
+        <v>549</v>
+      </c>
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
     </row>
     <row r="51" spans="1:19" ht="30" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
       <c r="H51" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="J51" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="K51" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="L51" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="M51" s="25" t="s">
         <v>345</v>
       </c>
-      <c r="L51" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="M51" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="15"/>
-      <c r="Q51" s="38" t="s">
-        <v>552</v>
-      </c>
-      <c r="R51" s="38"/>
-      <c r="S51" s="38"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="27"/>
+      <c r="Q51" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
     </row>
     <row r="52" spans="1:19" ht="30" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
       <c r="H52" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="J52" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="K52" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="L52" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="M52" s="25" t="s">
         <v>351</v>
       </c>
-      <c r="L52" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="M52" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="38" t="s">
-        <v>553</v>
-      </c>
-      <c r="R52" s="38"/>
-      <c r="S52" s="38"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="27"/>
+      <c r="Q52" s="16" t="s">
+        <v>551</v>
+      </c>
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
     </row>
     <row r="53" spans="1:19" ht="30" customHeight="1">
       <c r="A53" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B53" s="23" t="s">
+      <c r="B53" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
       <c r="H53" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="I53" s="2" t="s">
+      <c r="K53" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="L53" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="M53" s="25" t="s">
         <v>280</v>
       </c>
-      <c r="L53" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="M53" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="38" t="s">
-        <v>554</v>
-      </c>
-      <c r="R53" s="38"/>
-      <c r="S53" s="38"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
+      <c r="P53" s="27"/>
+      <c r="Q53" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
     </row>
     <row r="54" spans="1:19" ht="30" customHeight="1">
       <c r="A54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
       <c r="H54" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="K54" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="L54" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="M54" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="L54" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="M54" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="38" t="s">
-        <v>555</v>
-      </c>
-      <c r="R54" s="38"/>
-      <c r="S54" s="38"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="27"/>
+      <c r="Q54" s="16" t="s">
+        <v>553</v>
+      </c>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
     </row>
     <row r="55" spans="1:19" ht="30" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
       <c r="H55" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="I55" s="2" t="s">
+      <c r="K55" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="J55" s="2" t="s">
+      <c r="L55" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="M55" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="L55" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="M55" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="38" t="s">
-        <v>556</v>
-      </c>
-      <c r="R55" s="38"/>
-      <c r="S55" s="38"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="21"/>
+      <c r="P55" s="21"/>
+      <c r="Q55" s="16" t="s">
+        <v>554</v>
+      </c>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
     </row>
     <row r="56" spans="1:19" ht="30" customHeight="1">
       <c r="A56" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
       <c r="H56" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="I56" s="2" t="s">
+      <c r="K56" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="J56" s="2" t="s">
+      <c r="L56" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="M56" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="L56" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="M56" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="38" t="s">
-        <v>557</v>
-      </c>
-      <c r="R56" s="38"/>
-      <c r="S56" s="38"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="21"/>
+      <c r="Q56" s="16" t="s">
+        <v>555</v>
+      </c>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
     </row>
     <row r="57" spans="1:19" ht="30" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
       <c r="H57" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="K57" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="J57" s="2" t="s">
+      <c r="L57" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K57" s="2" t="s">
+      <c r="M57" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="L57" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="M57" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="38" t="s">
-        <v>558</v>
-      </c>
-      <c r="R57" s="38"/>
-      <c r="S57" s="38"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="21"/>
+      <c r="Q57" s="16" t="s">
+        <v>556</v>
+      </c>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
     </row>
     <row r="58" spans="1:19" ht="30" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
       <c r="H58" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I58" s="2" t="s">
+      <c r="K58" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="J58" s="2" t="s">
+      <c r="L58" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="K58" s="2" t="s">
+      <c r="M58" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="L58" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="M58" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="38" t="s">
-        <v>559</v>
-      </c>
-      <c r="R58" s="38"/>
-      <c r="S58" s="38"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="21"/>
+      <c r="P58" s="21"/>
+      <c r="Q58" s="16" t="s">
+        <v>557</v>
+      </c>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
     </row>
     <row r="59" spans="1:19" ht="30" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="23" t="s">
+      <c r="B59" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
       <c r="H59" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="J59" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="K59" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="L59" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="K59" s="2" t="s">
+      <c r="M59" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="L59" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="M59" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="38" t="s">
-        <v>560</v>
-      </c>
-      <c r="R59" s="38"/>
-      <c r="S59" s="38"/>
+      <c r="N59" s="21"/>
+      <c r="O59" s="21"/>
+      <c r="P59" s="21"/>
+      <c r="Q59" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
     </row>
     <row r="60" spans="1:19" ht="30" customHeight="1">
       <c r="A60" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
       <c r="H60" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="K60" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="L60" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="M60" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="L60" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="M60" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="38" t="s">
-        <v>561</v>
-      </c>
-      <c r="R60" s="38"/>
-      <c r="S60" s="38"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="21"/>
+      <c r="Q60" s="16" t="s">
+        <v>559</v>
+      </c>
+      <c r="R60" s="16"/>
+      <c r="S60" s="16"/>
     </row>
     <row r="61" spans="1:19" ht="30" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
       <c r="H61" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="K61" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="J61" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="M61" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="L61" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="M61" s="11" t="s">
-        <v>330</v>
-      </c>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="38" t="s">
-        <v>562</v>
-      </c>
-      <c r="R61" s="38"/>
-      <c r="S61" s="38"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="21"/>
+      <c r="Q61" s="16" t="s">
+        <v>560</v>
+      </c>
+      <c r="R61" s="16"/>
+      <c r="S61" s="16"/>
     </row>
     <row r="62" spans="1:19" ht="15.75">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="25"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="25"/>
-      <c r="L62" s="25"/>
-      <c r="M62" s="25"/>
-      <c r="N62" s="25"/>
-      <c r="S62" s="35"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="31"/>
+      <c r="K62" s="31"/>
+      <c r="L62" s="31"/>
+      <c r="M62" s="31"/>
+      <c r="N62" s="31"/>
+      <c r="S62" s="13"/>
     </row>
     <row r="63" spans="1:19" ht="16.5">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="33"/>
       <c r="H63" s="4" t="s">
         <v>74</v>
       </c>
@@ -6181,15 +6181,15 @@
       <c r="L63" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M63" s="12" t="s">
+      <c r="M63" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12"/>
-      <c r="P63" s="12"/>
+      <c r="N63" s="28"/>
+      <c r="O63" s="28"/>
+      <c r="P63" s="28"/>
       <c r="Q63" s="7"/>
-      <c r="R63" s="34" t="s">
-        <v>510</v>
+      <c r="R63" s="12" t="s">
+        <v>508</v>
       </c>
       <c r="S63" s="7"/>
     </row>
@@ -6197,684 +6197,684 @@
       <c r="A64" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="23" t="s">
+      <c r="B64" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="29"/>
       <c r="H64" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="K64" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="L64" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="K64" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="M64" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="38" t="s">
-        <v>563</v>
-      </c>
-      <c r="R64" s="38"/>
-      <c r="S64" s="38"/>
+      <c r="M64" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="N64" s="21"/>
+      <c r="O64" s="21"/>
+      <c r="P64" s="21"/>
+      <c r="Q64" s="16" t="s">
+        <v>561</v>
+      </c>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
     </row>
     <row r="65" spans="1:19" ht="30" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="23" t="s">
+      <c r="B65" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="23"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
       <c r="H65" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="J65" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="K65" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="L65" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="K65" s="2" t="s">
+      <c r="M65" s="21" t="s">
         <v>428</v>
       </c>
-      <c r="L65" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="M65" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="N65" s="11"/>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="38" t="s">
-        <v>564</v>
-      </c>
-      <c r="R65" s="38"/>
-      <c r="S65" s="38"/>
+      <c r="N65" s="21"/>
+      <c r="O65" s="21"/>
+      <c r="P65" s="21"/>
+      <c r="Q65" s="16" t="s">
+        <v>562</v>
+      </c>
+      <c r="R65" s="16"/>
+      <c r="S65" s="16"/>
     </row>
     <row r="66" spans="1:19" ht="30" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B66" s="23" t="s">
+      <c r="B66" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
       <c r="H66" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="J66" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="K66" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="L66" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="M66" s="21" t="s">
         <v>434</v>
       </c>
-      <c r="L66" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="M66" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="N66" s="11"/>
-      <c r="O66" s="11"/>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="38" t="s">
-        <v>565</v>
-      </c>
-      <c r="R66" s="38"/>
-      <c r="S66" s="38"/>
+      <c r="N66" s="21"/>
+      <c r="O66" s="21"/>
+      <c r="P66" s="21"/>
+      <c r="Q66" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="R66" s="16"/>
+      <c r="S66" s="16"/>
     </row>
     <row r="67" spans="1:19" ht="30" customHeight="1">
       <c r="A67" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
+      <c r="G67" s="29"/>
       <c r="H67" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="J67" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="K67" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="J67" s="2" t="s">
+      <c r="L67" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="K67" s="2" t="s">
+      <c r="M67" s="21" t="s">
         <v>440</v>
       </c>
-      <c r="L67" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="M67" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="N67" s="11"/>
-      <c r="O67" s="11"/>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="38" t="s">
-        <v>566</v>
-      </c>
-      <c r="R67" s="38"/>
-      <c r="S67" s="38"/>
+      <c r="N67" s="21"/>
+      <c r="O67" s="21"/>
+      <c r="P67" s="21"/>
+      <c r="Q67" s="16" t="s">
+        <v>564</v>
+      </c>
+      <c r="R67" s="16"/>
+      <c r="S67" s="16"/>
     </row>
     <row r="68" spans="1:19" ht="30" customHeight="1">
       <c r="A68" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29"/>
       <c r="H68" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="K68" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="L68" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="K68" s="2" t="s">
+      <c r="M68" s="21" t="s">
         <v>446</v>
       </c>
-      <c r="L68" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="M68" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="N68" s="11"/>
-      <c r="O68" s="11"/>
-      <c r="P68" s="11"/>
-      <c r="Q68" s="38" t="s">
-        <v>567</v>
-      </c>
-      <c r="R68" s="38"/>
-      <c r="S68" s="38"/>
+      <c r="N68" s="21"/>
+      <c r="O68" s="21"/>
+      <c r="P68" s="21"/>
+      <c r="Q68" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="R68" s="16"/>
+      <c r="S68" s="16"/>
     </row>
     <row r="69" spans="1:19" ht="30" customHeight="1">
       <c r="A69" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="23" t="s">
+      <c r="B69" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="23"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
       <c r="H69" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="J69" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="M69" s="21" t="s">
         <v>452</v>
       </c>
-      <c r="L69" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="M69" s="11" t="s">
-        <v>454</v>
-      </c>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="38" t="s">
-        <v>568</v>
-      </c>
-      <c r="R69" s="38"/>
-      <c r="S69" s="38"/>
+      <c r="N69" s="21"/>
+      <c r="O69" s="21"/>
+      <c r="P69" s="21"/>
+      <c r="Q69" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="R69" s="16"/>
+      <c r="S69" s="16"/>
     </row>
     <row r="70" spans="1:19" ht="30" customHeight="1">
       <c r="A70" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B70" s="23" t="s">
+      <c r="B70" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="23"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
       <c r="H70" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="J70" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="K70" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="L70" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="K70" s="2" t="s">
+      <c r="M70" s="21" t="s">
         <v>458</v>
       </c>
-      <c r="L70" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="M70" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="N70" s="11"/>
-      <c r="O70" s="11"/>
-      <c r="P70" s="11"/>
-      <c r="Q70" s="38" t="s">
-        <v>569</v>
-      </c>
-      <c r="R70" s="38"/>
-      <c r="S70" s="38"/>
+      <c r="N70" s="21"/>
+      <c r="O70" s="21"/>
+      <c r="P70" s="21"/>
+      <c r="Q70" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="R70" s="16"/>
+      <c r="S70" s="16"/>
     </row>
     <row r="71" spans="1:19" ht="30" customHeight="1">
       <c r="A71" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="23"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
       <c r="H71" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="J71" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="K71" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="L71" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="K71" s="2" t="s">
+      <c r="M71" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="L71" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="M71" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="N71" s="11"/>
-      <c r="O71" s="11"/>
-      <c r="P71" s="11"/>
-      <c r="Q71" s="38" t="s">
-        <v>570</v>
-      </c>
-      <c r="R71" s="38"/>
-      <c r="S71" s="38"/>
+      <c r="N71" s="21"/>
+      <c r="O71" s="21"/>
+      <c r="P71" s="21"/>
+      <c r="Q71" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
     </row>
     <row r="72" spans="1:19" ht="30" customHeight="1">
       <c r="A72" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B72" s="23" t="s">
+      <c r="B72" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="29"/>
       <c r="H72" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="J72" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="K72" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="M72" s="21" t="s">
         <v>470</v>
       </c>
-      <c r="L72" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="M72" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="N72" s="11"/>
-      <c r="O72" s="11"/>
-      <c r="P72" s="11"/>
-      <c r="Q72" s="38" t="s">
-        <v>571</v>
-      </c>
-      <c r="R72" s="38"/>
-      <c r="S72" s="38"/>
+      <c r="N72" s="21"/>
+      <c r="O72" s="21"/>
+      <c r="P72" s="21"/>
+      <c r="Q72" s="16" t="s">
+        <v>569</v>
+      </c>
+      <c r="R72" s="16"/>
+      <c r="S72" s="16"/>
     </row>
     <row r="73" spans="1:19" ht="30" customHeight="1">
       <c r="A73" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
       <c r="H73" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="K73" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="L73" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="M73" s="21" t="s">
         <v>476</v>
       </c>
-      <c r="L73" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="M73" s="11" t="s">
-        <v>478</v>
-      </c>
-      <c r="N73" s="11"/>
-      <c r="O73" s="11"/>
-      <c r="P73" s="11"/>
-      <c r="Q73" s="38" t="s">
-        <v>572</v>
-      </c>
-      <c r="R73" s="38"/>
-      <c r="S73" s="38"/>
+      <c r="N73" s="21"/>
+      <c r="O73" s="21"/>
+      <c r="P73" s="21"/>
+      <c r="Q73" s="16" t="s">
+        <v>570</v>
+      </c>
+      <c r="R73" s="16"/>
+      <c r="S73" s="16"/>
     </row>
     <row r="74" spans="1:19" ht="30" customHeight="1">
       <c r="A74" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B74" s="23" t="s">
+      <c r="B74" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
       <c r="H74" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="J74" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="L74" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="M74" s="21" t="s">
         <v>482</v>
       </c>
-      <c r="L74" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="M74" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
-      <c r="P74" s="11"/>
-      <c r="Q74" s="38" t="s">
-        <v>573</v>
-      </c>
-      <c r="R74" s="38"/>
-      <c r="S74" s="38"/>
+      <c r="N74" s="21"/>
+      <c r="O74" s="21"/>
+      <c r="P74" s="21"/>
+      <c r="Q74" s="16" t="s">
+        <v>571</v>
+      </c>
+      <c r="R74" s="16"/>
+      <c r="S74" s="16"/>
     </row>
     <row r="75" spans="1:19" ht="30" customHeight="1">
       <c r="A75" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B75" s="23" t="s">
+      <c r="B75" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="23"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
       <c r="H75" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="J75" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="K75" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="L75" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="M75" s="21" t="s">
         <v>488</v>
       </c>
-      <c r="L75" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="M75" s="11" t="s">
-        <v>490</v>
-      </c>
-      <c r="N75" s="11"/>
-      <c r="O75" s="11"/>
-      <c r="P75" s="11"/>
-      <c r="Q75" s="38" t="s">
-        <v>574</v>
-      </c>
-      <c r="R75" s="38"/>
-      <c r="S75" s="38"/>
+      <c r="N75" s="21"/>
+      <c r="O75" s="21"/>
+      <c r="P75" s="21"/>
+      <c r="Q75" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="R75" s="16"/>
+      <c r="S75" s="16"/>
     </row>
     <row r="76" spans="1:19" ht="30" customHeight="1">
       <c r="A76" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B76" s="23" t="s">
+      <c r="B76" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
       <c r="H76" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="J76" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="K76" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="L76" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="K76" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="M76" s="11" t="s">
-        <v>508</v>
-      </c>
-      <c r="N76" s="11"/>
-      <c r="O76" s="11"/>
-      <c r="P76" s="11"/>
-      <c r="Q76" s="38" t="s">
-        <v>575</v>
-      </c>
-      <c r="R76" s="38"/>
-      <c r="S76" s="38"/>
+      <c r="M76" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="N76" s="21"/>
+      <c r="O76" s="21"/>
+      <c r="P76" s="21"/>
+      <c r="Q76" s="16" t="s">
+        <v>573</v>
+      </c>
+      <c r="R76" s="16"/>
+      <c r="S76" s="16"/>
     </row>
     <row r="77" spans="1:19" ht="30" customHeight="1">
       <c r="A77" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B77" s="23" t="s">
+      <c r="B77" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
-      <c r="E77" s="23"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
       <c r="H77" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="J77" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="K77" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="L77" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="M77" s="21" t="s">
         <v>499</v>
       </c>
-      <c r="L77" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="M77" s="11" t="s">
-        <v>501</v>
-      </c>
-      <c r="N77" s="11"/>
-      <c r="O77" s="11"/>
-      <c r="P77" s="11"/>
-      <c r="Q77" s="38" t="s">
-        <v>576</v>
-      </c>
-      <c r="R77" s="38"/>
-      <c r="S77" s="38"/>
+      <c r="N77" s="21"/>
+      <c r="O77" s="21"/>
+      <c r="P77" s="21"/>
+      <c r="Q77" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="R77" s="16"/>
+      <c r="S77" s="16"/>
     </row>
     <row r="78" spans="1:19" ht="30" customHeight="1">
       <c r="A78" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="23" t="s">
+      <c r="B78" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C78" s="23"/>
-      <c r="D78" s="23"/>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
       <c r="H78" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="J78" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="K78" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="L78" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="M78" s="21" t="s">
         <v>505</v>
       </c>
-      <c r="L78" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="M78" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="N78" s="11"/>
-      <c r="O78" s="11"/>
-      <c r="P78" s="11"/>
-      <c r="Q78" s="38" t="s">
+      <c r="N78" s="21"/>
+      <c r="O78" s="21"/>
+      <c r="P78" s="21"/>
+      <c r="Q78" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="R78" s="16"/>
+      <c r="S78" s="16"/>
+    </row>
+    <row r="79" spans="1:19" ht="15.75">
+      <c r="A79" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="31"/>
+      <c r="I79" s="31"/>
+      <c r="J79" s="31"/>
+      <c r="K79" s="31"/>
+      <c r="L79" s="31"/>
+      <c r="M79" s="31"/>
+      <c r="N79" s="31"/>
+      <c r="S79" s="13"/>
+    </row>
+    <row r="80" spans="1:19" ht="15.75">
+      <c r="A80" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="38"/>
+      <c r="K80" s="38"/>
+      <c r="L80" s="38"/>
+      <c r="M80" s="38"/>
+      <c r="N80" s="38"/>
+      <c r="O80" s="38"/>
+      <c r="P80" s="38"/>
+      <c r="Q80" s="6"/>
+      <c r="R80" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="S80" s="15"/>
+    </row>
+    <row r="81" spans="1:19" ht="30" customHeight="1">
+      <c r="A81" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="36" t="s">
+        <v>576</v>
+      </c>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="36"/>
+      <c r="I81" s="36"/>
+      <c r="J81" s="36"/>
+      <c r="K81" s="36"/>
+      <c r="L81" s="36"/>
+      <c r="M81" s="36"/>
+      <c r="N81" s="36"/>
+      <c r="O81" s="36"/>
+      <c r="P81" s="36"/>
+      <c r="Q81" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="R81" s="16"/>
+      <c r="S81" s="16"/>
+    </row>
+    <row r="82" spans="1:19" ht="30" customHeight="1">
+      <c r="A82" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="R78" s="38"/>
-      <c r="S78" s="38"/>
-    </row>
-    <row r="79" spans="1:19" ht="15.75">
-      <c r="A79" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="25"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="25"/>
-      <c r="K79" s="25"/>
-      <c r="L79" s="25"/>
-      <c r="M79" s="25"/>
-      <c r="N79" s="25"/>
-      <c r="S79" s="35"/>
-    </row>
-    <row r="80" spans="1:19" ht="15.75">
-      <c r="A80" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="32"/>
-      <c r="H80" s="32"/>
-      <c r="I80" s="32"/>
-      <c r="J80" s="32"/>
-      <c r="K80" s="32"/>
-      <c r="L80" s="32"/>
-      <c r="M80" s="32"/>
-      <c r="N80" s="32"/>
-      <c r="O80" s="32"/>
-      <c r="P80" s="32"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="33" t="s">
-        <v>515</v>
-      </c>
-      <c r="S80" s="37"/>
-    </row>
-    <row r="81" spans="1:19" ht="30" customHeight="1">
-      <c r="A81" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="30" t="s">
-        <v>578</v>
-      </c>
-      <c r="E81" s="30"/>
-      <c r="F81" s="30"/>
-      <c r="G81" s="30"/>
-      <c r="H81" s="30"/>
-      <c r="I81" s="30"/>
-      <c r="J81" s="30"/>
-      <c r="K81" s="30"/>
-      <c r="L81" s="30"/>
-      <c r="M81" s="30"/>
-      <c r="N81" s="30"/>
-      <c r="O81" s="30"/>
-      <c r="P81" s="30"/>
-      <c r="Q81" s="38" t="s">
-        <v>580</v>
-      </c>
-      <c r="R81" s="38"/>
-      <c r="S81" s="38"/>
-    </row>
-    <row r="82" spans="1:19" ht="30" customHeight="1">
-      <c r="A82" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="30" t="s">
+      <c r="E82" s="36"/>
+      <c r="F82" s="36"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="36"/>
+      <c r="I82" s="36"/>
+      <c r="J82" s="36"/>
+      <c r="K82" s="36"/>
+      <c r="L82" s="36"/>
+      <c r="M82" s="36"/>
+      <c r="N82" s="36"/>
+      <c r="O82" s="36"/>
+      <c r="P82" s="36"/>
+      <c r="Q82" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30"/>
-      <c r="G82" s="30"/>
-      <c r="H82" s="30"/>
-      <c r="I82" s="30"/>
-      <c r="J82" s="30"/>
-      <c r="K82" s="30"/>
-      <c r="L82" s="30"/>
-      <c r="M82" s="30"/>
-      <c r="N82" s="30"/>
-      <c r="O82" s="30"/>
-      <c r="P82" s="30"/>
-      <c r="Q82" s="38" t="s">
-        <v>581</v>
-      </c>
-      <c r="R82" s="38"/>
-      <c r="S82" s="38"/>
+      <c r="R82" s="16"/>
+      <c r="S82" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="162">
@@ -6915,6 +6915,17 @@
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="M22:P22"/>
     <mergeCell ref="M26:P26"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="M30:P30"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B39:G39"/>
@@ -6938,6 +6949,9 @@
     <mergeCell ref="B44:G44"/>
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="B46:G46"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="M43:P43"/>
+    <mergeCell ref="M44:P44"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="B58:G58"/>
     <mergeCell ref="B59:G59"/>
@@ -6978,17 +6992,6 @@
     <mergeCell ref="M12:P12"/>
     <mergeCell ref="M13:P13"/>
     <mergeCell ref="M15:P15"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="M30:P30"/>
     <mergeCell ref="M31:P31"/>
     <mergeCell ref="M71:P71"/>
     <mergeCell ref="P2:S2"/>
@@ -7011,6 +7014,8 @@
     <mergeCell ref="M53:P53"/>
     <mergeCell ref="M54:P54"/>
     <mergeCell ref="M56:P56"/>
+    <mergeCell ref="M61:P61"/>
+    <mergeCell ref="M63:P63"/>
     <mergeCell ref="A82:C82"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
@@ -7035,11 +7040,6 @@
     <mergeCell ref="M58:P58"/>
     <mergeCell ref="M59:P59"/>
     <mergeCell ref="M60:P60"/>
-    <mergeCell ref="M61:P61"/>
-    <mergeCell ref="M63:P63"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="M43:P43"/>
-    <mergeCell ref="M44:P44"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>